<commit_message>
Plot of the data
</commit_message>
<xml_diff>
--- a/Supernova SN1993J/Data/Datos SuperNova.xlsx
+++ b/Supernova SN1993J/Data/Datos SuperNova.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1828" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1828" uniqueCount="24">
   <si>
     <t>Days from reference</t>
   </si>
@@ -89,9 +89,6 @@
   </si>
   <si>
     <t>Error</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Days </t>
   </si>
 </sst>
 </file>
@@ -201,7 +198,28 @@
   <cellStyles count="1">
     <cellStyle xfId="0" name="Normal" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="2">
+    <dxf>
+      <font/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB7E1CD"/>
+          <bgColor rgb="FFB7E1CD"/>
+        </patternFill>
+      </fill>
+      <border/>
+    </dxf>
+    <dxf>
+      <font/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFF0000"/>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+      <border/>
+    </dxf>
+  </dxfs>
 </styleSheet>
 </file>
 
@@ -21156,16 +21174,16 @@
       <c r="C133" s="10">
         <v>22.79</v>
       </c>
-      <c r="D133" s="8"/>
+      <c r="D133" s="8">
+        <v>2.751</v>
+      </c>
       <c r="E133" s="6">
-        <v>2.751</v>
-      </c>
-      <c r="F133" s="6">
         <v>103.65</v>
       </c>
-      <c r="G133" s="10">
+      <c r="F133" s="9">
         <v>5.202</v>
       </c>
+      <c r="G133" s="8"/>
       <c r="H133" s="8"/>
       <c r="I133" s="6"/>
       <c r="J133" s="9"/>
@@ -34767,7 +34785,7 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="17" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B1" s="18" t="s">
         <v>1</v>
@@ -34792,6 +34810,10 @@
       <c r="D2" s="18">
         <v>0.08</v>
       </c>
+      <c r="E2" s="18">
+        <f t="shared" ref="E2:E105" si="1">IF(C2&gt;D2,0,1)</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="18">
@@ -34806,6 +34828,10 @@
       <c r="D3" s="18">
         <v>0.052</v>
       </c>
+      <c r="E3" s="18">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="18">
@@ -34820,6 +34846,10 @@
       <c r="D4" s="18">
         <v>0.063</v>
       </c>
+      <c r="E4" s="18">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="18">
@@ -34834,6 +34864,10 @@
       <c r="D5" s="18">
         <v>0.074</v>
       </c>
+      <c r="E5" s="18">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" s="18">
@@ -34848,6 +34882,10 @@
       <c r="D6" s="18">
         <v>0.066</v>
       </c>
+      <c r="E6" s="18">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" s="18">
@@ -34862,6 +34900,10 @@
       <c r="D7" s="18">
         <v>0.095</v>
       </c>
+      <c r="E7" s="18">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" s="18">
@@ -34876,6 +34918,10 @@
       <c r="D8" s="18">
         <v>0.11</v>
       </c>
+      <c r="E8" s="18">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" s="18">
@@ -34890,6 +34936,10 @@
       <c r="D9" s="18">
         <v>0.113</v>
       </c>
+      <c r="E9" s="18">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" s="18">
@@ -34904,6 +34954,10 @@
       <c r="D10" s="18">
         <v>0.13</v>
       </c>
+      <c r="E10" s="18">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" s="18">
@@ -34918,6 +34972,10 @@
       <c r="D11" s="18">
         <v>0.149</v>
       </c>
+      <c r="E11" s="18">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" s="18">
@@ -34932,6 +34990,10 @@
       <c r="D12" s="18">
         <v>0.182</v>
       </c>
+      <c r="E12" s="18">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" s="18">
@@ -34946,6 +35008,10 @@
       <c r="D13" s="18">
         <v>0.178</v>
       </c>
+      <c r="E13" s="18">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" s="18">
@@ -34960,6 +35026,10 @@
       <c r="D14" s="18">
         <v>0.195</v>
       </c>
+      <c r="E14" s="18">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" s="18">
@@ -34974,6 +35044,10 @@
       <c r="D15" s="18">
         <v>0.238</v>
       </c>
+      <c r="E15" s="18">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" s="18">
@@ -34988,6 +35062,10 @@
       <c r="D16" s="18">
         <v>0.299</v>
       </c>
+      <c r="E16" s="18">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" s="18">
@@ -35002,6 +35080,10 @@
       <c r="D17" s="18">
         <v>0.327</v>
       </c>
+      <c r="E17" s="18">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" s="18">
@@ -35016,6 +35098,10 @@
       <c r="D18" s="18">
         <v>0.31</v>
       </c>
+      <c r="E18" s="18">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" s="18">
@@ -35030,6 +35116,10 @@
       <c r="D19" s="18">
         <v>0.406</v>
       </c>
+      <c r="E19" s="18">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" s="18">
@@ -35044,6 +35134,10 @@
       <c r="D20" s="18">
         <v>0.529</v>
       </c>
+      <c r="E20" s="18">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" s="18">
@@ -35058,6 +35152,10 @@
       <c r="D21" s="18">
         <v>0.785</v>
       </c>
+      <c r="E21" s="18">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22" s="18">
@@ -35072,6 +35170,10 @@
       <c r="D22" s="18">
         <v>0.915</v>
       </c>
+      <c r="E22" s="18">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="23">
       <c r="A23" s="18">
@@ -35086,6 +35188,10 @@
       <c r="D23" s="18">
         <v>1.11</v>
       </c>
+      <c r="E23" s="18">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="24">
       <c r="A24" s="18">
@@ -35100,6 +35206,10 @@
       <c r="D24" s="18">
         <v>1.298</v>
       </c>
+      <c r="E24" s="18">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="25">
       <c r="A25" s="18">
@@ -35114,6 +35224,10 @@
       <c r="D25" s="18">
         <v>1.734</v>
       </c>
+      <c r="E25" s="18">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="26">
       <c r="A26" s="18">
@@ -35128,6 +35242,10 @@
       <c r="D26" s="18">
         <v>2.007</v>
       </c>
+      <c r="E26" s="18">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="27">
       <c r="A27" s="18">
@@ -35142,6 +35260,10 @@
       <c r="D27" s="18">
         <v>2.22</v>
       </c>
+      <c r="E27" s="18">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="28">
       <c r="A28" s="18">
@@ -35156,6 +35278,10 @@
       <c r="D28" s="18">
         <v>2.82</v>
       </c>
+      <c r="E28" s="18">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="29">
       <c r="A29" s="18">
@@ -35170,6 +35296,10 @@
       <c r="D29" s="18">
         <v>3.572</v>
       </c>
+      <c r="E29" s="18">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="30">
       <c r="A30" s="18">
@@ -35184,6 +35314,10 @@
       <c r="D30" s="18">
         <v>4.018</v>
       </c>
+      <c r="E30" s="18">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="31">
       <c r="A31" s="18">
@@ -35198,6 +35332,10 @@
       <c r="D31" s="18">
         <v>4.379</v>
       </c>
+      <c r="E31" s="18">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="32">
       <c r="A32" s="18">
@@ -35212,6 +35350,10 @@
       <c r="D32" s="18">
         <v>5.142</v>
       </c>
+      <c r="E32" s="18">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="33">
       <c r="A33" s="18">
@@ -35226,6 +35368,10 @@
       <c r="D33" s="18">
         <v>5.583</v>
       </c>
+      <c r="E33" s="18">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="34">
       <c r="A34" s="18">
@@ -35240,6 +35386,10 @@
       <c r="D34" s="18">
         <v>5.223</v>
       </c>
+      <c r="E34" s="18">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="35">
       <c r="A35" s="18">
@@ -35254,6 +35404,10 @@
       <c r="D35" s="18">
         <v>5.539</v>
       </c>
+      <c r="E35" s="18">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="36">
       <c r="A36" s="18">
@@ -35268,6 +35422,10 @@
       <c r="D36" s="18">
         <v>6.236</v>
       </c>
+      <c r="E36" s="18">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="37">
       <c r="A37" s="18">
@@ -35282,6 +35440,10 @@
       <c r="D37" s="18">
         <v>5.66</v>
       </c>
+      <c r="E37" s="18">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="38">
       <c r="A38" s="18">
@@ -35296,6 +35458,10 @@
       <c r="D38" s="18">
         <v>5.523</v>
       </c>
+      <c r="E38" s="18">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="39">
       <c r="A39" s="18">
@@ -35310,6 +35476,10 @@
       <c r="D39" s="18">
         <v>5.971</v>
       </c>
+      <c r="E39" s="18">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="40">
       <c r="A40" s="18">
@@ -35324,6 +35494,10 @@
       <c r="D40" s="18">
         <v>5.925</v>
       </c>
+      <c r="E40" s="18">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="41">
       <c r="A41" s="18">
@@ -35338,6 +35512,10 @@
       <c r="D41" s="18">
         <v>6.057</v>
       </c>
+      <c r="E41" s="18">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="42">
       <c r="A42" s="18">
@@ -35352,6 +35530,10 @@
       <c r="D42" s="18">
         <v>5.62</v>
       </c>
+      <c r="E42" s="18">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="43">
       <c r="A43" s="18">
@@ -35360,11 +35542,15 @@
       <c r="B43" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="C43" s="18">
-        <v>2.751</v>
-      </c>
-      <c r="D43" s="18">
+      <c r="C43" s="6">
         <v>103.65</v>
+      </c>
+      <c r="D43" s="9">
+        <v>5.202</v>
+      </c>
+      <c r="E43" s="18">
+        <f t="shared" si="1"/>
+        <v>0</v>
       </c>
     </row>
     <row r="44">
@@ -35380,6 +35566,10 @@
       <c r="D44" s="18">
         <v>5.211</v>
       </c>
+      <c r="E44" s="18">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="45">
       <c r="A45" s="18">
@@ -35394,6 +35584,10 @@
       <c r="D45" s="18">
         <v>5.268</v>
       </c>
+      <c r="E45" s="18">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="46">
       <c r="A46" s="18">
@@ -35408,6 +35602,10 @@
       <c r="D46" s="18">
         <v>5.013</v>
       </c>
+      <c r="E46" s="18">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="47">
       <c r="A47" s="18">
@@ -35422,6 +35620,10 @@
       <c r="D47" s="18">
         <v>5.012</v>
       </c>
+      <c r="E47" s="18">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="48">
       <c r="A48" s="18">
@@ -35436,6 +35638,10 @@
       <c r="D48" s="18">
         <v>4.905</v>
       </c>
+      <c r="E48" s="18">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="49">
       <c r="A49" s="18">
@@ -35450,6 +35656,10 @@
       <c r="D49" s="18">
         <v>5.474</v>
       </c>
+      <c r="E49" s="18">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="50">
       <c r="A50" s="18">
@@ -35464,6 +35674,10 @@
       <c r="D50" s="18">
         <v>4.9</v>
       </c>
+      <c r="E50" s="18">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="51">
       <c r="A51" s="18">
@@ -35478,6 +35692,10 @@
       <c r="D51" s="18">
         <v>4.924</v>
       </c>
+      <c r="E51" s="18">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="52">
       <c r="A52" s="18">
@@ -35492,6 +35710,10 @@
       <c r="D52" s="18">
         <v>4.758</v>
       </c>
+      <c r="E52" s="18">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="53">
       <c r="A53" s="18">
@@ -35506,6 +35728,10 @@
       <c r="D53" s="18">
         <v>4.674</v>
       </c>
+      <c r="E53" s="18">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="54">
       <c r="A54" s="18">
@@ -35520,6 +35746,10 @@
       <c r="D54" s="18">
         <v>4.7</v>
       </c>
+      <c r="E54" s="18">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="55">
       <c r="A55" s="18">
@@ -35534,6 +35764,10 @@
       <c r="D55" s="18">
         <v>4.517</v>
       </c>
+      <c r="E55" s="18">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="56">
       <c r="A56" s="18">
@@ -35548,6 +35782,10 @@
       <c r="D56" s="18">
         <v>4.396</v>
       </c>
+      <c r="E56" s="18">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="57">
       <c r="A57" s="18">
@@ -35562,6 +35800,10 @@
       <c r="D57" s="18">
         <v>4.238</v>
       </c>
+      <c r="E57" s="18">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="58">
       <c r="A58" s="18">
@@ -35576,6 +35818,10 @@
       <c r="D58" s="18">
         <v>4.267</v>
       </c>
+      <c r="E58" s="18">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="59">
       <c r="A59" s="18">
@@ -35590,6 +35836,10 @@
       <c r="D59" s="18">
         <v>4.052</v>
       </c>
+      <c r="E59" s="18">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="60">
       <c r="A60" s="18">
@@ -35604,6 +35854,10 @@
       <c r="D60" s="18">
         <v>4.0</v>
       </c>
+      <c r="E60" s="18">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="61">
       <c r="A61" s="18">
@@ -35618,6 +35872,10 @@
       <c r="D61" s="18">
         <v>4.804</v>
       </c>
+      <c r="E61" s="18">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="62">
       <c r="A62" s="18">
@@ -35632,6 +35890,10 @@
       <c r="D62" s="18">
         <v>4.031</v>
       </c>
+      <c r="E62" s="18">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="63">
       <c r="A63" s="18">
@@ -35646,6 +35908,10 @@
       <c r="D63" s="18">
         <v>3.6</v>
       </c>
+      <c r="E63" s="18">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="64">
       <c r="A64" s="18">
@@ -35660,6 +35926,10 @@
       <c r="D64" s="18">
         <v>3.762</v>
       </c>
+      <c r="E64" s="18">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="65">
       <c r="A65" s="18">
@@ -35674,6 +35944,10 @@
       <c r="D65" s="18">
         <v>3.291</v>
       </c>
+      <c r="E65" s="18">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="66">
       <c r="A66" s="18">
@@ -35688,6 +35962,10 @@
       <c r="D66" s="18">
         <v>3.274</v>
       </c>
+      <c r="E66" s="18">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="67">
       <c r="A67" s="18">
@@ -35702,6 +35980,10 @@
       <c r="D67" s="18">
         <v>3.757</v>
       </c>
+      <c r="E67" s="18">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="68">
       <c r="A68" s="18">
@@ -35716,6 +35998,10 @@
       <c r="D68" s="18">
         <v>3.0</v>
       </c>
+      <c r="E68" s="18">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="69">
       <c r="A69" s="18">
@@ -35730,6 +36016,10 @@
       <c r="D69" s="18">
         <v>2.919</v>
       </c>
+      <c r="E69" s="18">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="70">
       <c r="A70" s="18">
@@ -35744,6 +36034,10 @@
       <c r="D70" s="18">
         <v>3.041</v>
       </c>
+      <c r="E70" s="18">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="71">
       <c r="A71" s="18">
@@ -35758,6 +36052,10 @@
       <c r="D71" s="18">
         <v>3.135</v>
       </c>
+      <c r="E71" s="18">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="72">
       <c r="A72" s="18">
@@ -35772,6 +36070,10 @@
       <c r="D72" s="18">
         <v>2.6</v>
       </c>
+      <c r="E72" s="18">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="73">
       <c r="A73" s="18">
@@ -35786,6 +36088,10 @@
       <c r="D73" s="18">
         <v>2.188</v>
       </c>
+      <c r="E73" s="18">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="74">
       <c r="A74" s="18">
@@ -35800,6 +36106,10 @@
       <c r="D74" s="18">
         <v>2.5</v>
       </c>
+      <c r="E74" s="18">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="75">
       <c r="A75" s="18">
@@ -35814,6 +36124,10 @@
       <c r="D75" s="18">
         <v>2.764</v>
       </c>
+      <c r="E75" s="18">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="76">
       <c r="A76" s="18">
@@ -35828,6 +36142,10 @@
       <c r="D76" s="18">
         <v>2.3</v>
       </c>
+      <c r="E76" s="18">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="77">
       <c r="A77" s="18">
@@ -35842,6 +36160,10 @@
       <c r="D77" s="18">
         <v>2.242</v>
       </c>
+      <c r="E77" s="18">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="78">
       <c r="A78" s="18">
@@ -35856,6 +36178,10 @@
       <c r="D78" s="18">
         <v>1.939</v>
       </c>
+      <c r="E78" s="18">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="79">
       <c r="A79" s="18">
@@ -35870,6 +36196,10 @@
       <c r="D79" s="18">
         <v>1.9</v>
       </c>
+      <c r="E79" s="18">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="80">
       <c r="A80" s="18">
@@ -35884,6 +36214,10 @@
       <c r="D80" s="18">
         <v>1.965</v>
       </c>
+      <c r="E80" s="18">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="81">
       <c r="A81" s="18">
@@ -35898,6 +36232,10 @@
       <c r="D81" s="18">
         <v>1.7</v>
       </c>
+      <c r="E81" s="18">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="82">
       <c r="A82" s="18">
@@ -35912,6 +36250,10 @@
       <c r="D82" s="18">
         <v>1.696</v>
       </c>
+      <c r="E82" s="18">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="83">
       <c r="A83" s="18">
@@ -35926,6 +36268,10 @@
       <c r="D83" s="18">
         <v>1.6</v>
       </c>
+      <c r="E83" s="18">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="84">
       <c r="A84" s="18">
@@ -35940,6 +36286,10 @@
       <c r="D84" s="18">
         <v>1.4</v>
       </c>
+      <c r="E84" s="18">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="85">
       <c r="A85" s="18">
@@ -35954,6 +36304,10 @@
       <c r="D85" s="18">
         <v>1.434</v>
       </c>
+      <c r="E85" s="18">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="86">
       <c r="A86" s="18">
@@ -35968,6 +36322,10 @@
       <c r="D86" s="18">
         <v>1.4</v>
       </c>
+      <c r="E86" s="18">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="87">
       <c r="A87" s="18">
@@ -35982,6 +36340,10 @@
       <c r="D87" s="18">
         <v>1.573</v>
       </c>
+      <c r="E87" s="18">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="88">
       <c r="A88" s="18">
@@ -35996,6 +36358,10 @@
       <c r="D88" s="18">
         <v>1.3</v>
       </c>
+      <c r="E88" s="18">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="89">
       <c r="A89" s="18">
@@ -36010,6 +36376,10 @@
       <c r="D89" s="18">
         <v>1.3</v>
       </c>
+      <c r="E89" s="18">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="90">
       <c r="A90" s="18">
@@ -36024,6 +36394,10 @@
       <c r="D90" s="18">
         <v>1.3</v>
       </c>
+      <c r="E90" s="18">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="91">
       <c r="A91" s="18">
@@ -36038,6 +36412,10 @@
       <c r="D91" s="18">
         <v>1.136</v>
       </c>
+      <c r="E91" s="18">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="92">
       <c r="A92" s="18">
@@ -36052,6 +36430,10 @@
       <c r="D92" s="18">
         <v>1.1</v>
       </c>
+      <c r="E92" s="18">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="93">
       <c r="A93" s="18">
@@ -36066,6 +36448,10 @@
       <c r="D93" s="18">
         <v>1.0</v>
       </c>
+      <c r="E93" s="18">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="94">
       <c r="A94" s="18">
@@ -36080,6 +36466,10 @@
       <c r="D94" s="17">
         <v>0.927</v>
       </c>
+      <c r="E94" s="18">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="95">
       <c r="A95" s="18">
@@ -36094,6 +36484,10 @@
       <c r="D95" s="17">
         <v>1.2</v>
       </c>
+      <c r="E95" s="18">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="96">
       <c r="A96" s="18">
@@ -36108,6 +36502,10 @@
       <c r="D96" s="17">
         <v>0.9</v>
       </c>
+      <c r="E96" s="18">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="97">
       <c r="A97" s="18">
@@ -36122,6 +36520,10 @@
       <c r="D97" s="18">
         <v>0.4</v>
       </c>
+      <c r="E97" s="18">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="98">
       <c r="A98" s="18">
@@ -36136,6 +36538,10 @@
       <c r="D98" s="17">
         <v>0.7</v>
       </c>
+      <c r="E98" s="18">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="99">
       <c r="A99" s="18">
@@ -36150,6 +36556,10 @@
       <c r="D99" s="18">
         <v>0.774</v>
       </c>
+      <c r="E99" s="18">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="100">
       <c r="A100" s="18">
@@ -36164,6 +36574,10 @@
       <c r="D100" s="18">
         <v>0.429</v>
       </c>
+      <c r="E100" s="18">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="101">
       <c r="A101" s="18">
@@ -36178,6 +36592,10 @@
       <c r="D101" s="18">
         <v>0.424</v>
       </c>
+      <c r="E101" s="18">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="102">
       <c r="A102" s="18">
@@ -36192,6 +36610,10 @@
       <c r="D102" s="18">
         <v>0.376</v>
       </c>
+      <c r="E102" s="18">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="103">
       <c r="A103" s="18">
@@ -36206,6 +36628,10 @@
       <c r="D103" s="18">
         <v>0.304</v>
       </c>
+      <c r="E103" s="18">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="104">
       <c r="A104" s="18">
@@ -36220,6 +36646,10 @@
       <c r="D104" s="18">
         <v>0.276</v>
       </c>
+      <c r="E104" s="18">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="105">
       <c r="A105" s="17">
@@ -36234,8 +36664,22 @@
       <c r="D105" s="18">
         <v>0.48</v>
       </c>
+      <c r="E105" s="18">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="E1:E1000">
+    <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="0">
+      <formula>NOT(ISERROR(SEARCH(("0"),(E1))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E1:E1000">
+    <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="1">
+      <formula>NOT(ISERROR(SEARCH(("1"),(E1))))</formula>
+    </cfRule>
+  </conditionalFormatting>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>

</xml_diff>